<commit_message>
Edit company detail screen.
</commit_message>
<xml_diff>
--- a/01_document/DB定義書.xlsx
+++ b/01_document/DB定義書.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="667" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="667" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="テーブル一覧" sheetId="24" r:id="rId1"/>
@@ -378,16 +378,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>担当者氏名</t>
-    <rPh sb="0" eb="3">
-      <t>タントウシャ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>担当者部署1</t>
     <rPh sb="0" eb="3">
       <t>タントウシャ</t>
@@ -803,13 +793,6 @@
   </si>
   <si>
     <t>企業名かな</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>担当者かな</t>
-    <rPh sb="0" eb="3">
-      <t>タントウシャ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1050,10 +1033,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>employee_first_name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>create_user</t>
   </si>
   <si>
@@ -1213,14 +1192,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>person_in_charge</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>person_in_charge_kana</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>department_in_charge1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1581,10 +1552,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>employee_last_name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1874,6 +1841,42 @@
   </si>
   <si>
     <t>ビル名</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>担当者姓</t>
+    <rPh sb="0" eb="3">
+      <t>タントウシャ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>担当者名</t>
+    <rPh sb="0" eb="3">
+      <t>タントウシャ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>employee_last_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>person_in_charge_last_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>employee_first_name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>person_in_charge_first_name</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2525,16 +2528,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1">
@@ -2543,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C2" s="35" t="str">
         <f>企業マスタ!$B$2</f>
@@ -2560,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C3" s="36" t="str">
         <f>従業員マスタ!$B$2</f>
@@ -2577,7 +2580,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C4" s="36" t="str">
         <f>従業員パスワードマスタ!$B$2</f>
@@ -2594,7 +2597,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C5" s="36" t="str">
         <f>評価方式マスタ!$B$2</f>
@@ -2611,7 +2614,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C6" s="36" t="str">
         <f>メール設定マスタ!$B$2</f>
@@ -2628,7 +2631,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C7" s="36" t="str">
         <f>質問グループマスタ!$B$2</f>
@@ -2645,7 +2648,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C8" s="36" t="str">
         <f>質問グループサブマスタ!$B$2</f>
@@ -2662,7 +2665,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C9" s="36" t="str">
         <f>質問マスタ!$B$2</f>
@@ -2679,7 +2682,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C10" s="36" t="str">
         <f>評価者社内マスタ!$B$2</f>
@@ -2696,7 +2699,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C11" s="42" t="str">
         <f>評価者社外マスタ!$B$2</f>
@@ -2713,7 +2716,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C12" s="35" t="str">
         <f>お知らせデータ!$B$2</f>
@@ -2730,7 +2733,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C13" s="36" t="str">
         <f>メール送信データ!$B$2</f>
@@ -2747,7 +2750,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="C14" s="36" t="str">
         <f>評価結果データ!$B$2</f>
@@ -2824,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -2833,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -2871,7 +2874,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -2889,13 +2892,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -2908,7 +2911,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -2918,13 +2921,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -2943,13 +2946,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -2968,13 +2971,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -2993,13 +2996,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E12" s="26" t="s">
         <v>13</v>
@@ -3011,7 +3014,7 @@
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -3020,13 +3023,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
@@ -3038,7 +3041,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -3047,13 +3050,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -3065,7 +3068,7 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -3077,10 +3080,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>13</v>
@@ -3102,17 +3105,17 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>14</v>
@@ -3126,13 +3129,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="4">
         <v>125</v>
@@ -3152,10 +3155,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -3172,13 +3175,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="4">
         <v>125</v>
@@ -3198,10 +3201,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -3245,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -3254,7 +3257,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -3292,7 +3295,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -3310,13 +3313,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -3329,7 +3332,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -3339,13 +3342,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -3370,7 +3373,7 @@
         <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -3389,13 +3392,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="4">
         <v>50</v>
@@ -3414,13 +3417,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="4">
         <v>50</v>
@@ -3439,13 +3442,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="18">
         <v>100</v>
@@ -3464,13 +3467,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E14" s="18">
         <v>100</v>
@@ -3487,13 +3490,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="18">
         <v>50</v>
@@ -3510,13 +3513,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E16" s="17">
         <v>255</v>
@@ -3535,13 +3538,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>13</v>
@@ -3553,7 +3556,7 @@
       </c>
       <c r="I17" s="27"/>
       <c r="J17" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -3562,13 +3565,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -3580,7 +3583,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -3589,13 +3592,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>13</v>
@@ -3607,7 +3610,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -3619,10 +3622,10 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -3644,17 +3647,17 @@
         <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>14</v>
@@ -3668,13 +3671,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E22" s="4">
         <v>125</v>
@@ -3694,10 +3697,10 @@
         <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
@@ -3714,13 +3717,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E24" s="4">
         <v>125</v>
@@ -3740,10 +3743,10 @@
         <v>16</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -3822,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -3831,7 +3834,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -3845,7 +3848,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -3869,7 +3872,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -3887,13 +3890,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -3916,13 +3919,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E9" s="4">
         <v>255</v>
@@ -3944,17 +3947,17 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>14</v>
@@ -3968,13 +3971,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="4">
         <v>125</v>
@@ -3994,10 +3997,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -4014,13 +4017,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>125</v>
@@ -4040,10 +4043,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -4086,7 +4089,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -4095,7 +4098,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -4109,7 +4112,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -4133,7 +4136,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -4151,13 +4154,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -4180,13 +4183,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -4205,13 +4208,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E10" s="4">
         <v>255</v>
@@ -4230,13 +4233,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="4">
         <v>50</v>
@@ -4255,13 +4258,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="4">
         <v>500</v>
@@ -4280,13 +4283,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
@@ -4298,7 +4301,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -4307,13 +4310,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -4332,13 +4335,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>13</v>
@@ -4358,17 +4361,17 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>14</v>
@@ -4382,13 +4385,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="4">
         <v>125</v>
@@ -4408,10 +4411,10 @@
         <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -4428,13 +4431,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="4">
         <v>125</v>
@@ -4454,10 +4457,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -4500,7 +4503,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -4509,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -4547,7 +4550,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -4565,13 +4568,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -4594,13 +4597,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -4622,10 +4625,10 @@
         <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -4644,13 +4647,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -4669,13 +4672,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -4687,7 +4690,7 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="39.6">
@@ -4696,13 +4699,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>13</v>
@@ -4714,7 +4717,7 @@
       </c>
       <c r="I13" s="27"/>
       <c r="J13" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -4723,13 +4726,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -4741,7 +4744,7 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -4753,10 +4756,10 @@
         <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>13</v>
@@ -4775,13 +4778,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -4793,7 +4796,7 @@
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -4802,13 +4805,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>13</v>
@@ -4827,13 +4830,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E18" s="4">
         <v>50</v>
@@ -4855,10 +4858,10 @@
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="4">
         <v>100</v>
@@ -4877,13 +4880,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -4902,16 +4905,16 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -4930,17 +4933,17 @@
         <v>17</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>14</v>
@@ -4954,13 +4957,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E23" s="4">
         <v>125</v>
@@ -4980,10 +4983,10 @@
         <v>15</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>13</v>
@@ -5000,13 +5003,13 @@
         <v>18</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E25" s="4">
         <v>125</v>
@@ -5026,10 +5029,10 @@
         <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>13</v>
@@ -5050,9 +5053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
@@ -5081,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -5119,7 +5120,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -5137,13 +5138,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>18</v>
@@ -5166,13 +5167,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E9" s="44">
         <v>25</v>
@@ -5194,10 +5195,10 @@
         <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E10" s="18">
         <v>50</v>
@@ -5216,13 +5217,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="18">
         <v>50</v>
@@ -5244,10 +5245,10 @@
         <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="18">
         <v>20</v>
@@ -5266,13 +5267,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="18">
         <v>125</v>
@@ -5284,7 +5285,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="1" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5293,13 +5294,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E14" s="18">
         <v>125</v>
@@ -5311,7 +5312,7 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -5320,13 +5321,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="18">
         <v>125</v>
@@ -5338,7 +5339,7 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -5350,10 +5351,10 @@
         <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E16" s="18">
         <v>20</v>
@@ -5372,16 +5373,16 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>294</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>175</v>
+        <v>297</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="18">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -5397,21 +5398,21 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>117</v>
+        <v>295</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>176</v>
+        <v>299</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E18" s="18">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="1"/>
@@ -5422,13 +5423,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="18">
         <v>100</v>
@@ -5447,13 +5448,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E20" s="18">
         <v>100</v>
@@ -5470,13 +5471,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E21" s="18">
         <v>50</v>
@@ -5493,13 +5494,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E22" s="18">
         <v>255</v>
@@ -5521,24 +5522,24 @@
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>38</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -5547,13 +5548,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E24" s="4">
         <v>125</v>
@@ -5573,10 +5574,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>36</v>
@@ -5593,13 +5594,13 @@
         <v>19</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E26" s="4">
         <v>125</v>
@@ -5619,10 +5620,10 @@
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>36</v>
@@ -5647,8 +5648,8 @@
   </sheetPr>
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -5678,7 +5679,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -5692,7 +5693,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -5716,7 +5717,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -5734,13 +5735,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>18</v>
@@ -5766,10 +5767,10 @@
         <v>34</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E9" s="4">
         <v>50</v>
@@ -5781,7 +5782,7 @@
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K9" s="19"/>
     </row>
@@ -5791,13 +5792,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -5816,13 +5817,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -5841,13 +5842,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="4">
         <v>50</v>
@@ -5866,13 +5867,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>149</v>
+        <v>298</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>50</v>
@@ -5891,13 +5892,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E14" s="18">
         <v>100</v>
@@ -5916,13 +5917,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="18">
         <v>100</v>
@@ -5939,13 +5940,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E16" s="18">
         <v>50</v>
@@ -5962,16 +5963,16 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -5987,13 +5988,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E18" s="17">
         <v>255</v>
@@ -6018,7 +6019,7 @@
         <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="4">
         <v>30</v>
@@ -6042,17 +6043,17 @@
         <v>17</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>19</v>
@@ -6066,13 +6067,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E21" s="4">
         <v>125</v>
@@ -6092,10 +6093,10 @@
         <v>15</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>36</v>
@@ -6112,13 +6113,13 @@
         <v>16</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E23" s="4">
         <v>125</v>
@@ -6138,10 +6139,10 @@
         <v>16</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>36</v>
@@ -6184,7 +6185,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -6193,7 +6194,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -6207,7 +6208,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C5" s="8"/>
     </row>
@@ -6231,7 +6232,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -6249,13 +6250,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -6276,24 +6277,24 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -6309,7 +6310,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E10" s="17">
         <v>250</v>
@@ -6328,13 +6329,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="4">
         <v>125</v>
@@ -6354,10 +6355,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>36</v>
@@ -6374,13 +6375,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>125</v>
@@ -6400,10 +6401,10 @@
         <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>36</v>
@@ -6445,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -6454,7 +6455,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -6468,7 +6469,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -6492,7 +6493,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -6510,13 +6511,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -6539,13 +6540,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -6564,13 +6565,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -6582,7 +6583,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -6591,13 +6592,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -6609,7 +6610,7 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -6618,13 +6619,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -6636,7 +6637,7 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -6645,13 +6646,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
@@ -6663,7 +6664,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -6672,13 +6673,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -6690,7 +6691,7 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -6699,13 +6700,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>13</v>
@@ -6717,7 +6718,7 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -6726,13 +6727,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -6744,7 +6745,7 @@
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -6753,13 +6754,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>13</v>
@@ -6771,7 +6772,7 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6780,13 +6781,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -6798,7 +6799,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -6807,13 +6808,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>13</v>
@@ -6825,7 +6826,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -6834,13 +6835,13 @@
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -6852,7 +6853,7 @@
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -6861,13 +6862,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>13</v>
@@ -6879,7 +6880,7 @@
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -6888,13 +6889,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>13</v>
@@ -6906,7 +6907,7 @@
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -6918,17 +6919,17 @@
         <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>14</v>
@@ -6942,13 +6943,13 @@
         <v>17</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E24" s="4">
         <v>125</v>
@@ -6968,10 +6969,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>13</v>
@@ -6988,13 +6989,13 @@
         <v>19</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E26" s="4">
         <v>125</v>
@@ -7014,10 +7015,10 @@
         <v>16</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>13</v>
@@ -7060,7 +7061,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -7069,7 +7070,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -7083,7 +7084,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C5" s="14"/>
     </row>
@@ -7107,7 +7108,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -7125,13 +7126,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -7154,13 +7155,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -7179,13 +7180,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -7197,7 +7198,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -7206,13 +7207,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -7224,7 +7225,7 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7233,13 +7234,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="4">
         <v>50</v>
@@ -7258,13 +7259,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>500</v>
@@ -7286,17 +7287,17 @@
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>14</v>
@@ -7310,13 +7311,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="4">
         <v>125</v>
@@ -7336,10 +7337,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -7356,13 +7357,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="4">
         <v>125</v>
@@ -7382,10 +7383,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -7436,7 +7437,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -7474,7 +7475,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -7495,10 +7496,10 @@
         <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -7521,13 +7522,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>13</v>
@@ -7546,13 +7547,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E10" s="1">
         <v>100</v>
@@ -7571,13 +7572,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="1">
         <v>100</v>
@@ -7597,17 +7598,17 @@
         <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>14</v>
@@ -7621,13 +7622,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>125</v>
@@ -7647,10 +7648,10 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
@@ -7667,13 +7668,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="4">
         <v>125</v>
@@ -7693,10 +7694,10 @@
         <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -7739,7 +7740,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -7748,7 +7749,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -7786,7 +7787,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -7804,13 +7805,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -7833,13 +7834,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>13</v>
@@ -7861,10 +7862,10 @@
         <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>13</v>
@@ -7883,13 +7884,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>13</v>
@@ -7901,7 +7902,7 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -7910,13 +7911,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>13</v>
@@ -7928,7 +7929,7 @@
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="12" customFormat="1">
@@ -7937,16 +7938,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>135</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>137</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
@@ -7955,7 +7956,7 @@
       </c>
       <c r="I13" s="11"/>
       <c r="J13" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -7967,17 +7968,17 @@
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -7989,13 +7990,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="4">
         <v>125</v>
@@ -8015,10 +8016,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>13</v>
@@ -8035,13 +8036,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="4">
         <v>125</v>
@@ -8061,10 +8062,10 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
@@ -8106,7 +8107,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -8115,7 +8116,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="2"/>
@@ -8153,7 +8154,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>8</v>
@@ -8171,13 +8172,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>13</v>
@@ -8200,13 +8201,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -8218,7 +8219,7 @@
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -8227,13 +8228,13 @@
         <v>3</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E10" s="4">
         <v>50</v>
@@ -8258,7 +8259,7 @@
         <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E11" s="4">
         <v>100</v>
@@ -8277,13 +8278,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -8302,13 +8303,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E13" s="4">
         <v>20</v>
@@ -8327,13 +8328,13 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E14" s="4">
         <v>20</v>
@@ -8352,13 +8353,13 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E15" s="4">
         <v>20</v>
@@ -8377,13 +8378,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E16" s="4">
         <v>20</v>
@@ -8402,13 +8403,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="D17" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E17" s="4">
         <v>20</v>
@@ -8430,17 +8431,17 @@
         <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>14</v>
@@ -8454,13 +8455,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E19" s="4">
         <v>125</v>
@@ -8480,10 +8481,10 @@
         <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>13</v>
@@ -8500,13 +8501,13 @@
         <v>14</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E21" s="4">
         <v>125</v>
@@ -8526,10 +8527,10 @@
         <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>13</v>

</xml_diff>